<commit_message>
fix #140 utterance true turn to boolean
</commit_message>
<xml_diff>
--- a/test/spreadsheets/Voxa Cli Intents Utterances-only-alexa en-US.xlsx
+++ b/test/spreadsheets/Voxa Cli Intents Utterances-only-alexa en-US.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INTENT" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="102">
   <si>
     <t xml:space="preserve">Intent</t>
   </si>
@@ -153,6 +153,9 @@
     <t xml:space="preserve">Fallback skill</t>
   </si>
   <si>
+    <t xml:space="preserve">AMAZON.YesIntent</t>
+  </si>
+  <si>
     <t xml:space="preserve">JokeIntent</t>
   </si>
   <si>
@@ -174,10 +177,16 @@
     <t xml:space="preserve">I like {bear}</t>
   </si>
   <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
     <t xml:space="preserve">i want to travel from {originCity}</t>
   </si>
   <si>
     <t xml:space="preserve">I like {bear} bears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">i'm traveling from {originCity} to {destinationCity}</t>
@@ -334,11 +343,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -426,12 +436,6 @@
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans Mono"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="9">
@@ -636,11 +640,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -754,17 +758,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.3515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.37890625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.58"/>
@@ -963,7 +967,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="S9" s="0" t="s">
@@ -971,6 +975,11 @@
       </c>
       <c r="T9" s="0" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -989,12 +998,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.30078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1013,10 +1022,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>26</v>
@@ -1024,70 +1033,79 @@
       <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>43</v>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D6" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D7" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D9" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D10" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D11" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +1132,7 @@
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.83"/>
   </cols>
@@ -1126,17 +1144,17 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1173,22 +1191,22 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1229,7 +1247,7 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1265,26 +1283,26 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1320,7 +1338,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
@@ -1328,18 +1346,18 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1366,7 +1384,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35"/>
@@ -1375,24 +1393,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,11 +1426,11 @@
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1439,7 +1457,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="42.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="47.57"/>
@@ -1449,61 +1467,61 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix #140 utterance true turn to boolean (#141)
</commit_message>
<xml_diff>
--- a/test/spreadsheets/Voxa Cli Intents Utterances-only-alexa en-US.xlsx
+++ b/test/spreadsheets/Voxa Cli Intents Utterances-only-alexa en-US.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INTENT" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="102">
   <si>
     <t xml:space="preserve">Intent</t>
   </si>
@@ -153,6 +153,9 @@
     <t xml:space="preserve">Fallback skill</t>
   </si>
   <si>
+    <t xml:space="preserve">AMAZON.YesIntent</t>
+  </si>
+  <si>
     <t xml:space="preserve">JokeIntent</t>
   </si>
   <si>
@@ -174,10 +177,16 @@
     <t xml:space="preserve">I like {bear}</t>
   </si>
   <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
     <t xml:space="preserve">i want to travel from {originCity}</t>
   </si>
   <si>
     <t xml:space="preserve">I like {bear} bears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">i'm traveling from {originCity} to {destinationCity}</t>
@@ -334,11 +343,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -426,12 +436,6 @@
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans Mono"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="9">
@@ -636,11 +640,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -754,17 +758,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.3515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.37890625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.58"/>
@@ -963,7 +967,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="S9" s="0" t="s">
@@ -971,6 +975,11 @@
       </c>
       <c r="T9" s="0" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -989,12 +998,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.30078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1013,10 +1022,10 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>26</v>
@@ -1024,70 +1033,79 @@
       <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>43</v>
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D6" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D7" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D9" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D10" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D11" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1114,7 +1132,7 @@
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.83"/>
   </cols>
@@ -1126,17 +1144,17 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1173,22 +1191,22 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1229,7 +1247,7 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1265,26 +1283,26 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1320,7 +1338,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
@@ -1328,18 +1346,18 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1366,7 +1384,7 @@
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35"/>
@@ -1375,24 +1393,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,11 +1426,11 @@
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1439,7 +1457,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="42.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="47.57"/>
@@ -1449,61 +1467,61 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>